<commit_message>
add code nhanh Minh
</commit_message>
<xml_diff>
--- a/TaiLieu/ButtonDefinition.xlsx
+++ b/TaiLieu/ButtonDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\01.SmarTrack\TaiLieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CAE3C3-D279-4D67-B731-609B072289D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B34E477-8B0B-4BA6-87A3-97538F7B78C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>Màn hình sản xuất có đơn hàng</t>
   </si>
   <si>
-    <t>Bấm Refesh Màn hình sản xuất khi có chọn đơn hàng</t>
-  </si>
-  <si>
     <t>Tự động Refesh Màn hình sản xuất khi có chọn đơn hàng</t>
   </si>
   <si>
@@ -217,6 +214,9 @@
   </si>
   <si>
     <t>Gửi mail cho SendSupervisor</t>
+  </si>
+  <si>
+    <t>Refesh Màn hình sản xuất khi có chọn đơn hàng</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +552,7 @@
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="41.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="44.5703125" customWidth="1"/>
+    <col min="4" max="4" width="69.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -563,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -602,13 +602,13 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -664,7 +664,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
         <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -717,10 +717,10 @@
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
         <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -731,10 +731,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -742,13 +742,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -756,13 +756,13 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -770,13 +770,13 @@
         <v>140</v>
       </c>
       <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
         <v>26</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -784,13 +784,13 @@
         <v>170</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -798,13 +798,13 @@
         <v>200</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -812,13 +812,13 @@
         <v>100</v>
       </c>
       <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
         <v>33</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>34</v>
-      </c>
-      <c r="D19" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -826,13 +826,13 @@
         <v>101</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
         <v>36</v>
-      </c>
-      <c r="D20" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -840,13 +840,13 @@
         <v>70</v>
       </c>
       <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
         <v>38</v>
       </c>
-      <c r="C21" t="s">
-        <v>39</v>
-      </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -854,13 +854,13 @@
         <v>110</v>
       </c>
       <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
         <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -868,13 +868,13 @@
         <v>112</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -882,13 +882,13 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -896,13 +896,13 @@
         <v>300</v>
       </c>
       <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
         <v>46</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>47</v>
-      </c>
-      <c r="D25" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -910,13 +910,13 @@
         <v>301</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" t="s">
         <v>49</v>
-      </c>
-      <c r="D26" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -924,13 +924,13 @@
         <v>600</v>
       </c>
       <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
         <v>51</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>52</v>
-      </c>
-      <c r="D27" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -938,13 +938,13 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -952,13 +952,13 @@
         <v>303</v>
       </c>
       <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
         <v>61</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>62</v>
-      </c>
-      <c r="D29" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>